<commit_message>
First functioning version with small CxSystem2 hack in physiology_reference.py line 85 self._comparts_tmp2 -> self._comparts_tmp1
</commit_message>
<xml_diff>
--- a/MacV1Buildup/tables/post_syn_compartments.xlsx
+++ b/MacV1Buildup/tables/post_syn_compartments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simo\Laskenta\Git_Repos\CxConstructor\MacV1Buildup\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE94191-279D-41EE-8C75-1246EA121458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9178AF-9B8D-4131-9EB5-F097A253A5C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E7AC5DF3-BE1D-4C5A-9ADC-F9581D743E1F}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>ab</t>
   </si>
   <si>
-    <t>soma</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
@@ -98,10 +95,13 @@
     <t>0, 1, 0, 0, 0</t>
   </si>
   <si>
-    <t>0, 1, 0, 0, 1</t>
-  </si>
-  <si>
     <t>Soma Layer Target (FYI)</t>
+  </si>
+  <si>
+    <t>soma, nearestDendrite</t>
+  </si>
+  <si>
+    <t>.33, .33, .33, 1, 1</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,10 +483,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -497,16 +497,16 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -517,64 +517,64 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>